<commit_message>
first debug of training data implementation
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="7">
   <si>
     <t>Country</t>
   </si>
@@ -425,7 +425,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow for social care provision and alignment with social care receipt
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="7">
   <si>
     <t>Country</t>
   </si>
@@ -425,7 +425,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debug options.txt file for multi-run simulation
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="8">
   <si>
     <t>Country</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>2012</t>
+  </si>
+  <si>
+    <t>2019</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
calibration for care analysis
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="8">
   <si>
     <t>Country</t>
   </si>
@@ -428,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct problems in projection of social care
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="8">
   <si>
     <t>Country</t>
   </si>
@@ -428,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix tax donor database to facilitate use with alternative countries
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="8">
   <si>
     <t>Country</t>
   </si>
@@ -428,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update input parameters to correct specification
</commit_message>
<xml_diff>
--- a/input/DatabaseCountryYear.xlsx
+++ b/input/DatabaseCountryYear.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="8">
   <si>
     <t>Country</t>
   </si>
@@ -428,7 +428,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>